<commit_message>
Add forward fill for 'Region' column in unconstrained inventory DataFrame
</commit_message>
<xml_diff>
--- a/Discovery_Unconstrained_Sales Inventory Summary_2025-11-20-11-37-09.xlsx
+++ b/Discovery_Unconstrained_Sales Inventory Summary_2025-11-20-11-37-09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Projects\lucid_replica\production-planning-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7220E5CB-4833-46F3-97E1-16E1768BCE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987E3120-DA7C-402E-9A95-74BAF38BA9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>